<commit_message>
work with main sheet
</commit_message>
<xml_diff>
--- a/printers.xlsx
+++ b/printers.xlsx
@@ -12,16 +12,16 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
   </bookViews>
   <sheets>
-    <sheet name="MAIN" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="MAIN" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
     <sheet name="AL75023437" sheetId="3" r:id="rId3"/>
-    <sheet name="CNB1L7J286" sheetId="10" r:id="rId4"/>
-    <sheet name="VCF7538360" sheetId="4" r:id="rId5"/>
-    <sheet name="E75373J7N561836" sheetId="5" r:id="rId6"/>
-    <sheet name="VCG8Y01076" sheetId="6" r:id="rId7"/>
-    <sheet name="VCG9118770" sheetId="7" r:id="rId8"/>
-    <sheet name="VCG8887941" sheetId="8" r:id="rId9"/>
-    <sheet name="ZDP1BJFF9000RLT" sheetId="9" r:id="rId10"/>
+    <sheet name="CNB1L7J286" sheetId="4" r:id="rId4"/>
+    <sheet name="VCF7538360" sheetId="5" r:id="rId5"/>
+    <sheet name="E75373J7N561836" sheetId="6" r:id="rId6"/>
+    <sheet name="VCG8Y01076" sheetId="7" r:id="rId7"/>
+    <sheet name="VCG9118770" sheetId="8" r:id="rId8"/>
+    <sheet name="VCG8887941" sheetId="9" r:id="rId9"/>
+    <sheet name="ZDP1BJFF9000RLT" sheetId="10" r:id="rId10"/>
     <sheet name="Лист10" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -29,7 +29,106 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="88">
+  <si>
+    <t>Комната</t>
+  </si>
+  <si>
+    <t>Серийный номер</t>
+  </si>
+  <si>
+    <t>IP</t>
+  </si>
+  <si>
+    <t>Процент тонера</t>
+  </si>
+  <si>
+    <t>Последяя замена</t>
+  </si>
+  <si>
+    <t>Ожидаемое время замены</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>AL75023437</t>
+  </si>
+  <si>
+    <t>10.2.126.1</t>
+  </si>
+  <si>
+    <t>CNB1L7J286</t>
+  </si>
+  <si>
+    <t>10.2.124.4</t>
+  </si>
+  <si>
+    <t>E75198L1N182781</t>
+  </si>
+  <si>
+    <t>10.2.124.57</t>
+  </si>
+  <si>
+    <t>E75373J7N561817</t>
+  </si>
+  <si>
+    <t>10.2.124.56</t>
+  </si>
+  <si>
+    <t>E75373J7N561836</t>
+  </si>
+  <si>
+    <t>10.2.124.253</t>
+  </si>
+  <si>
+    <t>VCF7538360</t>
+  </si>
+  <si>
+    <t>10.2.125.23</t>
+  </si>
+  <si>
+    <t>VCG8887941</t>
+  </si>
+  <si>
+    <t>10.2.124.172</t>
+  </si>
+  <si>
+    <t>VCG8Y01076</t>
+  </si>
+  <si>
+    <t>10.2.124.208</t>
+  </si>
+  <si>
+    <t>VCG9118770</t>
+  </si>
+  <si>
+    <t>10.2.124.199</t>
+  </si>
+  <si>
+    <t>ZDP1BJAF80005JJ</t>
+  </si>
+  <si>
+    <t>10.2.124.45</t>
+  </si>
+  <si>
+    <t>ZDP1BJFF9000RLT</t>
+  </si>
+  <si>
+    <t>10.2.124.132</t>
+  </si>
+  <si>
+    <t>ZDP1BJFF9000TJP</t>
+  </si>
+  <si>
+    <t>10.2.124.58</t>
+  </si>
+  <si>
+    <t>ZDP1BJFF9000VXY</t>
+  </si>
+  <si>
+    <t>10.2.124.15</t>
+  </si>
   <si>
     <t>Название</t>
   </si>
@@ -37,15 +136,6 @@
     <t>Модель</t>
   </si>
   <si>
-    <t>IP</t>
-  </si>
-  <si>
-    <t>Комната</t>
-  </si>
-  <si>
-    <t>Серийный номер</t>
-  </si>
-  <si>
     <t>Цвет тонера</t>
   </si>
   <si>
@@ -58,21 +148,9 @@
     <t>Кол-во напечатанных страниц</t>
   </si>
   <si>
-    <t>Процент тонера</t>
-  </si>
-  <si>
     <t>MC853-VENERA</t>
   </si>
   <si>
-    <t>10.2.126.1</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>AL75023437</t>
-  </si>
-  <si>
     <t>black</t>
   </si>
   <si>
@@ -85,18 +163,54 @@
     <t>39321</t>
   </si>
   <si>
+    <t>KONTRAK</t>
+  </si>
+  <si>
+    <t>HP LaserJet MFP M435nda</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>33722</t>
+  </si>
+  <si>
+    <t>BRNB422005D0F93</t>
+  </si>
+  <si>
+    <t>Brother MFC-L2700DN</t>
+  </si>
+  <si>
+    <t>-2</t>
+  </si>
+  <si>
+    <t>-3</t>
+  </si>
+  <si>
+    <t>330</t>
+  </si>
+  <si>
+    <t>BRN3C2AF42EF82D</t>
+  </si>
+  <si>
+    <t>Brother DCP-L5500DN</t>
+  </si>
+  <si>
+    <t>17574</t>
+  </si>
+  <si>
+    <t>BRN3C2AF42EF755</t>
+  </si>
+  <si>
+    <t>6444</t>
+  </si>
+  <si>
     <t>KM33F7E9</t>
   </si>
   <si>
     <t>Kyocera MFP httpd 0.0.1</t>
   </si>
   <si>
-    <t>10.2.125.23</t>
-  </si>
-  <si>
-    <t>VCF7538360</t>
-  </si>
-  <si>
     <t>7200</t>
   </si>
   <si>
@@ -106,36 +220,18 @@
     <t>12121</t>
   </si>
   <si>
-    <t>BRN3C2AF42EF755</t>
-  </si>
-  <si>
-    <t>Brother DCP-L5500DN</t>
-  </si>
-  <si>
-    <t>10.2.124.253</t>
-  </si>
-  <si>
-    <t>E75373J7N561836</t>
-  </si>
-  <si>
-    <t>-2</t>
-  </si>
-  <si>
-    <t>-3</t>
-  </si>
-  <si>
-    <t>6444</t>
+    <t>KM767774</t>
+  </si>
+  <si>
+    <t>4680</t>
+  </si>
+  <si>
+    <t>15148</t>
   </si>
   <si>
     <t>M2540dn-514kab</t>
   </si>
   <si>
-    <t>10.2.124.208</t>
-  </si>
-  <si>
-    <t>VCG8Y01076</t>
-  </si>
-  <si>
     <t>2160</t>
   </si>
   <si>
@@ -145,12 +241,6 @@
     <t>KM7B9F0D</t>
   </si>
   <si>
-    <t>10.2.124.199</t>
-  </si>
-  <si>
-    <t>VCG9118770</t>
-  </si>
-  <si>
     <t>3600</t>
   </si>
   <si>
@@ -160,19 +250,19 @@
     <t>783</t>
   </si>
   <si>
-    <t>KM767774</t>
-  </si>
-  <si>
-    <t>10.2.124.172</t>
-  </si>
-  <si>
-    <t>VCG8887941</t>
-  </si>
-  <si>
-    <t>4680</t>
-  </si>
-  <si>
-    <t>15148</t>
+    <t>SEC30CDA73402B9</t>
+  </si>
+  <si>
+    <t>Samsung M337x</t>
+  </si>
+  <si>
+    <t>10000</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>54738</t>
   </si>
   <si>
     <t>SEC30CDA737D7A3</t>
@@ -181,18 +271,6 @@
     <t>Samsung M337x 407x</t>
   </si>
   <si>
-    <t>10.2.124.132</t>
-  </si>
-  <si>
-    <t>ZDP1BJFF9000RLT</t>
-  </si>
-  <si>
-    <t>Black</t>
-  </si>
-  <si>
-    <t>10000</t>
-  </si>
-  <si>
     <t>3200</t>
   </si>
   <si>
@@ -202,100 +280,19 @@
     <t>SEC30CDA737D7BF</t>
   </si>
   <si>
-    <t>10.2.124.58</t>
-  </si>
-  <si>
-    <t>ZDP1BJFF9000TJP</t>
-  </si>
-  <si>
     <t>200</t>
   </si>
   <si>
     <t>60605</t>
   </si>
   <si>
-    <t>BRNB422005D0F93</t>
-  </si>
-  <si>
-    <t>Brother MFC-L2700DN</t>
-  </si>
-  <si>
-    <t>10.2.124.57</t>
-  </si>
-  <si>
-    <t>E75198L1N182781</t>
-  </si>
-  <si>
-    <t>330</t>
-  </si>
-  <si>
-    <t>BRN3C2AF42EF82D</t>
-  </si>
-  <si>
-    <t>10.2.124.56</t>
-  </si>
-  <si>
-    <t>E75373J7N561817</t>
-  </si>
-  <si>
-    <t>17574</t>
-  </si>
-  <si>
-    <t>SEC30CDA73402B9</t>
-  </si>
-  <si>
-    <t>Samsung M337x</t>
-  </si>
-  <si>
-    <t>10.2.124.45</t>
-  </si>
-  <si>
-    <t>ZDP1BJAF80005JJ</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>54738</t>
-  </si>
-  <si>
     <t>SEC30CDA737D7DA</t>
   </si>
   <si>
-    <t>10.2.124.15</t>
-  </si>
-  <si>
-    <t>ZDP1BJFF9000VXY</t>
-  </si>
-  <si>
     <t>3400</t>
   </si>
   <si>
     <t>41331</t>
-  </si>
-  <si>
-    <t>KONTRAK</t>
-  </si>
-  <si>
-    <t>HP LaserJet MFP M435nda</t>
-  </si>
-  <si>
-    <t>10.2.124.4</t>
-  </si>
-  <si>
-    <t>CNB1L7J286</t>
-  </si>
-  <si>
-    <t>33722</t>
-  </si>
-  <si>
-    <t>Ожидаемое время замены</t>
-  </si>
-  <si>
-    <t>Последяя замена</t>
-  </si>
-  <si>
-    <t>Серийний номер</t>
   </si>
 </sst>
 </file>
@@ -371,10 +368,10 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -390,6 +387,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -699,236 +699,302 @@
   <sheetPr>
     <tabColor theme="6"/>
   </sheetPr>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="16.5703125" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" customWidth="1"/>
-    <col min="5" max="5" width="25.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" customWidth="1"/>
+    <col min="6" max="6" width="25.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="7">
+        <v>0.39</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="7">
+        <v>0.39</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="D4" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1" t="s">
-        <v>12</v>
+      <c r="C5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="7">
+        <v>1.5</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="7">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="7">
+        <v>0.65</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="7">
+        <v>0.71</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="7">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" t="s">
-        <v>51</v>
-      </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1" t="s">
-        <v>12</v>
+      <c r="D12" s="7">
+        <v>0.32</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1" t="s">
-        <v>12</v>
+        <v>29</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="7">
+        <v>0.02</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1" t="s">
-        <v>12</v>
+        <v>31</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="7">
+        <v>0.34</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:E14">
-    <sortCondition ref="B2"/>
-  </sortState>
   <hyperlinks>
     <hyperlink ref="B2" location="AL75023437!A1" display="AL75023437"/>
     <hyperlink ref="B3" location="CNB1L7J286!A1" display="CNB1L7J286"/>
@@ -950,34 +1016,34 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -997,34 +1063,34 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -1039,8 +1105,8 @@
   </sheetPr>
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1058,469 +1124,466 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="J2" s="2">
-        <f>H2/G2</f>
+        <f t="shared" ref="J2:J14" si="0">H2/G2</f>
         <v>0.39</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>81</v>
+        <v>44</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>82</v>
+        <v>45</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>84</v>
+        <v>9</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>85</v>
+        <v>47</v>
       </c>
       <c r="J3" s="2">
-        <f>H3/G3</f>
+        <f t="shared" si="0"/>
         <v>0.39</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>63</v>
+        <v>12</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>64</v>
+        <v>11</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="J4" s="2">
-        <f>H4/G4</f>
+        <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>67</v>
+        <v>14</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>68</v>
+        <v>13</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="J5" s="2">
-        <f>H5/G5</f>
+        <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>25</v>
+        <v>56</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="J6" s="2">
-        <f>H6/G6</f>
+        <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="D7" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>22</v>
+        <v>60</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>24</v>
+        <v>62</v>
       </c>
       <c r="J7" s="2">
-        <f>H7/G7</f>
+        <f t="shared" si="0"/>
         <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="F8" s="1" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>22</v>
+        <v>60</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="J8" s="2">
-        <f>H8/G8</f>
+        <f t="shared" si="0"/>
         <v>0.65</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>32</v>
+        <v>66</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>22</v>
+        <v>60</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>35</v>
+        <v>67</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>36</v>
+        <v>68</v>
       </c>
       <c r="J9" s="2">
-        <f>H9/G9</f>
+        <f t="shared" si="0"/>
         <v>0.3</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>37</v>
+        <v>69</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>41</v>
+        <v>71</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="J10" s="2">
-        <f>H10/G10</f>
+        <f t="shared" si="0"/>
         <v>0.71</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>72</v>
+        <v>26</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>73</v>
+        <v>25</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>53</v>
+        <v>75</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="J11" s="2">
-        <f>H11/G11</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>48</v>
+        <v>78</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>49</v>
+        <v>79</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>53</v>
+        <v>75</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>54</v>
+        <v>80</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>55</v>
+        <v>81</v>
       </c>
       <c r="J12" s="2">
-        <f>H12/G12</f>
+        <f t="shared" si="0"/>
         <v>0.32</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>56</v>
+        <v>82</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>49</v>
+        <v>79</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>58</v>
+        <v>29</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>53</v>
+        <v>75</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="J13" s="2">
-        <f>H13/G13</f>
+        <f t="shared" si="0"/>
         <v>0.02</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>77</v>
+        <v>32</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>78</v>
+        <v>31</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>53</v>
+        <v>75</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="J14" s="2">
-        <f>H14/G14</f>
+        <f t="shared" si="0"/>
         <v>0.34</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:J14">
-    <sortCondition ref="E2"/>
-  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
@@ -1550,93 +1613,71 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="J2" s="2">
-        <f t="shared" ref="J2" si="0">H2/G2</f>
+        <f>H2/G2</f>
         <v>0.39</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
-      <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-        <x14:sparklineGroup displayEmptyCellsAs="gap">
-          <x14:colorSeries rgb="FF376092"/>
-          <x14:colorNegative rgb="FFD00000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FFD00000"/>
-          <x14:colorFirst rgb="FFD00000"/>
-          <x14:colorLast rgb="FFD00000"/>
-          <x14:colorHigh rgb="FFD00000"/>
-          <x14:colorLow rgb="FFD00000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>AL75023437!J2:J7</xm:f>
-              <xm:sqref>D11</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-      </x14:sparklineGroups>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1655,63 +1696,63 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>81</v>
+        <v>44</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>82</v>
+        <v>45</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>84</v>
+        <v>9</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>85</v>
+        <v>47</v>
       </c>
       <c r="J2" s="2">
         <f>H2/G2</f>
@@ -1749,66 +1790,66 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="D2" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>22</v>
+        <v>60</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>24</v>
+        <v>62</v>
       </c>
       <c r="J2" s="2">
-        <f t="shared" ref="J2" si="0">H2/G2</f>
+        <f>H2/G2</f>
         <v>0.55000000000000004</v>
       </c>
     </row>
@@ -1829,34 +1870,34 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -1876,34 +1917,34 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -1923,34 +1964,34 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -1970,34 +2011,34 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>